<commit_message>
Breaking EZ Interface API and operand behavior change. EZ Interface make_operand now must always accept a key and optionally a value and constraints. Parse code now will ignore option_descriptions what that do not have either unpack_option and mapped_key set. That is, if no mapped_key is set on an operand, then it will be ignored by the parser. This is actually more consistant with other code and the intent of the removed code was more for completeness rather than actually being a use case. Updated all test cases and examples.
</commit_message>
<xml_diff>
--- a/cmd_options.xlsx
+++ b/cmd_options.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tegtmeye/src/general/lemma/cmd_options/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tegtmeye/src/general/cmd_options/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24400" yWindow="6660" windowWidth="13800" windowHeight="17200" tabRatio="500"/>
+    <workbookView xWindow="24820" yWindow="7740" windowWidth="12900" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
   <si>
     <t>extended_description</t>
   </si>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,14 +718,16 @@
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="E14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
       <c r="J14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="6"/>
+      <c r="K14" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
@@ -736,10 +738,9 @@
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="2"/>
       <c r="J15" s="6" t="s">
         <v>14</v>
       </c>
@@ -750,135 +751,31 @@
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
-      <c r="P15" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4"/>
-      <c r="J16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="4"/>
-      <c r="J17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="2"/>
-      <c r="J18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="J19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="2"/>
-      <c r="J20" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="J21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" t="s">
+      <c r="P15" s="6"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" t="s">
         <v>11</v>
       </c>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" t="s">
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added mapped_key to EZ interface option spec. Updated test cases.
</commit_message>
<xml_diff>
--- a/cmd_options.xlsx
+++ b/cmd_options.xlsx
@@ -53,9 +53,6 @@
     <t>interpret_value</t>
   </si>
   <si>
-    <t>unpack_argument</t>
-  </si>
-  <si>
     <t>mapped_key</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>operand</t>
+  </si>
+  <si>
+    <t>unpack_option</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -436,13 +436,13 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="133" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -457,19 +457,19 @@
         <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>5</v>
@@ -488,7 +488,7 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
@@ -501,11 +501,11 @@
       <c r="F3" s="2"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
@@ -520,10 +520,10 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -536,13 +536,13 @@
       <c r="F5" s="2"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
@@ -560,11 +560,11 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O6" s="6"/>
       <c r="P6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.2">
@@ -575,16 +575,16 @@
       <c r="G7" s="2"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O7" s="6"/>
       <c r="P7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.2">
@@ -597,15 +597,15 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O8" s="6"/>
       <c r="P8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
@@ -616,18 +616,18 @@
       <c r="G9" s="2"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M9" s="6"/>
       <c r="N9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O9" s="6"/>
       <c r="P9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.2">
@@ -644,10 +644,10 @@
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
@@ -659,16 +659,16 @@
       <c r="H11" s="5"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
@@ -682,15 +682,15 @@
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
@@ -702,18 +702,18 @@
       <c r="H13" s="5"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
@@ -723,17 +723,17 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
       <c r="J14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
@@ -742,10 +742,10 @@
       <c r="E15" s="4"/>
       <c r="F15" s="2"/>
       <c r="J15" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
@@ -756,7 +756,7 @@
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -770,7 +770,7 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added feature to allow implicit values when value is not specified in the options_description.
</commit_message>
<xml_diff>
--- a/cmd_options.xlsx
+++ b/cmd_options.xlsx
@@ -426,7 +426,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,6 +484,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="5"/>
       <c r="F2" s="2"/>
+      <c r="G2" s="5"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -499,6 +500,7 @@
       <c r="C3" s="3"/>
       <c r="D3" s="2"/>
       <c r="F3" s="2"/>
+      <c r="G3" s="5"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
         <v>13</v>
@@ -517,6 +519,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="5"/>
       <c r="F4" s="2"/>
+      <c r="G4" s="5"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6" t="s">
@@ -534,6 +537,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="F5" s="2"/>
+      <c r="G5" s="5"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
         <v>13</v>

</xml_diff>